<commit_message>
Add another Palmerston North Field expt
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/PalmerstonNorth1989.xlsx
+++ b/Tests/Validation/Wheat/PalmerstonNorth1989.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="35">
   <si>
     <t>SimulationName</t>
   </si>
@@ -100,6 +100,36 @@
   <si>
     <t>PalmerstonNorth1989Sow5-AprCultivarRongotea</t>
   </si>
+  <si>
+    <t>PalmerstonNorth1994Sow22-DecCultivarBattenWinter</t>
+  </si>
+  <si>
+    <t>PalmerstonNorth1994Sow22-DecCultivarBattenSpring</t>
+  </si>
+  <si>
+    <t>PalmerstonNorth1994Sow27-OctCultivarBattenWinter</t>
+  </si>
+  <si>
+    <t>PalmerstonNorth1994Sow27-OctCultivarBattenSpring</t>
+  </si>
+  <si>
+    <t>PalmerstonNorth1994Sow1-SepCultivarBattenWinter</t>
+  </si>
+  <si>
+    <t>PalmerstonNorth1994Sow1-SepCultivarBattenSpring</t>
+  </si>
+  <si>
+    <t>PalmerstonNorth1994Sow20-JunCultivarBattenWinter</t>
+  </si>
+  <si>
+    <t>PalmerstonNorth1994Sow20-JunCultivarBattenSpring</t>
+  </si>
+  <si>
+    <t>PalmerstonNorth1994Sow5-AprCultivarBattenWinter</t>
+  </si>
+  <si>
+    <t>PalmerstonNorth1994Sow5-AprCultivarBattenSpring</t>
+  </si>
 </sst>
 </file>
 
@@ -108,13 +138,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -133,13 +168,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:G290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B281" sqref="B281:G290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,6 +2399,1639 @@
         <v>6</v>
       </c>
     </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>25</v>
+      </c>
+      <c r="B137" s="1">
+        <v>34704</v>
+      </c>
+      <c r="C137">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>25</v>
+      </c>
+      <c r="B138" s="1">
+        <v>34711</v>
+      </c>
+      <c r="C138">
+        <v>3.0500000000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>25</v>
+      </c>
+      <c r="B139" s="1">
+        <v>34715</v>
+      </c>
+      <c r="C139">
+        <v>3.8899999999999997</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>25</v>
+      </c>
+      <c r="B140" s="1">
+        <v>34718</v>
+      </c>
+      <c r="C140">
+        <v>4.3650000000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>25</v>
+      </c>
+      <c r="B141" s="1">
+        <v>34723</v>
+      </c>
+      <c r="C141">
+        <v>5.0631578947368414</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>25</v>
+      </c>
+      <c r="B142" s="1">
+        <v>34725</v>
+      </c>
+      <c r="C142">
+        <v>5.7312500000000002</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>25</v>
+      </c>
+      <c r="B143" s="1">
+        <v>34729</v>
+      </c>
+      <c r="C143">
+        <v>6.3812499999999988</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>25</v>
+      </c>
+      <c r="B144" s="1">
+        <v>34733</v>
+      </c>
+      <c r="C144">
+        <v>6.9866666666666664</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>25</v>
+      </c>
+      <c r="B145" s="1">
+        <v>34737</v>
+      </c>
+      <c r="C145">
+        <v>7.5866666666666669</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>25</v>
+      </c>
+      <c r="B146" s="1">
+        <v>34740</v>
+      </c>
+      <c r="C146">
+        <v>8.06</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>25</v>
+      </c>
+      <c r="B147" s="1">
+        <v>34744</v>
+      </c>
+      <c r="C147">
+        <v>8.7066666666666688</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>25</v>
+      </c>
+      <c r="B148" s="1">
+        <v>34751</v>
+      </c>
+      <c r="C148">
+        <v>9.7714285714285705</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>25</v>
+      </c>
+      <c r="B149" s="1">
+        <v>34754</v>
+      </c>
+      <c r="C149">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>25</v>
+      </c>
+      <c r="B150" s="1">
+        <v>34759</v>
+      </c>
+      <c r="C150">
+        <v>10.592857142857143</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>25</v>
+      </c>
+      <c r="B151" s="1">
+        <v>34765</v>
+      </c>
+      <c r="C151">
+        <v>11.142857142857144</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>25</v>
+      </c>
+      <c r="B152" s="1">
+        <v>34775</v>
+      </c>
+      <c r="C152">
+        <v>12.035714285714286</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>25</v>
+      </c>
+      <c r="B153" s="1">
+        <v>34785</v>
+      </c>
+      <c r="C153">
+        <v>12.958333333333334</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>25</v>
+      </c>
+      <c r="B154" s="1">
+        <v>34799</v>
+      </c>
+      <c r="C154">
+        <v>14.246153846153845</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>25</v>
+      </c>
+      <c r="B155" s="1">
+        <v>34807</v>
+      </c>
+      <c r="C155">
+        <v>14.899999999999999</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>25</v>
+      </c>
+      <c r="B156" s="1">
+        <v>34829</v>
+      </c>
+      <c r="C156">
+        <v>16.683333333333334</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>25</v>
+      </c>
+      <c r="B157" s="1">
+        <v>34838</v>
+      </c>
+      <c r="C157">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>26</v>
+      </c>
+      <c r="B158" s="1">
+        <v>34704</v>
+      </c>
+      <c r="C158">
+        <v>1.8249999999999997</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>26</v>
+      </c>
+      <c r="B159" s="1">
+        <v>34711</v>
+      </c>
+      <c r="C159">
+        <v>3.1450000000000005</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>26</v>
+      </c>
+      <c r="B160" s="1">
+        <v>34715</v>
+      </c>
+      <c r="C160">
+        <v>4.0349999999999993</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>26</v>
+      </c>
+      <c r="B161" s="1">
+        <v>34718</v>
+      </c>
+      <c r="C161">
+        <v>4.4999999999999991</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>26</v>
+      </c>
+      <c r="B162" s="1">
+        <v>34723</v>
+      </c>
+      <c r="C162">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>26</v>
+      </c>
+      <c r="B163" s="1">
+        <v>34725</v>
+      </c>
+      <c r="C163">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>26</v>
+      </c>
+      <c r="B164" s="1">
+        <v>34729</v>
+      </c>
+      <c r="C164">
+        <v>6.5421052631578949</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>26</v>
+      </c>
+      <c r="B165" s="1">
+        <v>34733</v>
+      </c>
+      <c r="C165">
+        <v>6.9555555555555557</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>26</v>
+      </c>
+      <c r="B166" s="1">
+        <v>34737</v>
+      </c>
+      <c r="C166">
+        <v>7.2625000000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>27</v>
+      </c>
+      <c r="B167" s="1">
+        <v>34655</v>
+      </c>
+      <c r="C167">
+        <v>2.9450000000000003</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>27</v>
+      </c>
+      <c r="B168" s="1">
+        <v>34659</v>
+      </c>
+      <c r="C168">
+        <v>3.5450000000000004</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>27</v>
+      </c>
+      <c r="B169" s="1">
+        <v>34662</v>
+      </c>
+      <c r="C169">
+        <v>4.1100000000000003</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>27</v>
+      </c>
+      <c r="B170" s="1">
+        <v>34666</v>
+      </c>
+      <c r="C170">
+        <v>4.9949999999999992</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>27</v>
+      </c>
+      <c r="B171" s="1">
+        <v>34669</v>
+      </c>
+      <c r="C171">
+        <v>5.4950000000000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>27</v>
+      </c>
+      <c r="B172" s="1">
+        <v>34675</v>
+      </c>
+      <c r="C172">
+        <v>6.7117647058823522</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>27</v>
+      </c>
+      <c r="B173" s="1">
+        <v>34682</v>
+      </c>
+      <c r="C173">
+        <v>7.7529411764705873</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>27</v>
+      </c>
+      <c r="B174" s="1">
+        <v>34687</v>
+      </c>
+      <c r="C174">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>27</v>
+      </c>
+      <c r="B175" s="1">
+        <v>34690</v>
+      </c>
+      <c r="C175">
+        <v>9.4764705882352906</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>27</v>
+      </c>
+      <c r="B176" s="1">
+        <v>34694</v>
+      </c>
+      <c r="C176">
+        <v>10.013333333333334</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>27</v>
+      </c>
+      <c r="B177" s="1">
+        <v>34697</v>
+      </c>
+      <c r="C177">
+        <v>10.45</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>27</v>
+      </c>
+      <c r="B178" s="1">
+        <v>34701</v>
+      </c>
+      <c r="C178">
+        <v>11.015384615384615</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>27</v>
+      </c>
+      <c r="B179" s="1">
+        <v>34704</v>
+      </c>
+      <c r="C179">
+        <v>11.266666666666666</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>27</v>
+      </c>
+      <c r="B180" s="1">
+        <v>34711</v>
+      </c>
+      <c r="C180">
+        <v>12.033333333333333</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>27</v>
+      </c>
+      <c r="B181" s="1">
+        <v>34725</v>
+      </c>
+      <c r="C181">
+        <v>14.455555555555557</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>27</v>
+      </c>
+      <c r="B182" s="1">
+        <v>34733</v>
+      </c>
+      <c r="C182">
+        <v>15.714285714285714</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>28</v>
+      </c>
+      <c r="B183" s="1">
+        <v>34655</v>
+      </c>
+      <c r="C183">
+        <v>2.6949999999999998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>28</v>
+      </c>
+      <c r="B184" s="1">
+        <v>34659</v>
+      </c>
+      <c r="C184">
+        <v>3.2789473684210524</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>28</v>
+      </c>
+      <c r="B185" s="1">
+        <v>34662</v>
+      </c>
+      <c r="C185">
+        <v>3.8249999999999993</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>28</v>
+      </c>
+      <c r="B186" s="1">
+        <v>34666</v>
+      </c>
+      <c r="C186">
+        <v>4.7150000000000007</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>28</v>
+      </c>
+      <c r="B187" s="1">
+        <v>34669</v>
+      </c>
+      <c r="C187">
+        <v>5.1850000000000005</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>28</v>
+      </c>
+      <c r="B188" s="1">
+        <v>34675</v>
+      </c>
+      <c r="C188">
+        <v>6.2111111111111112</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>28</v>
+      </c>
+      <c r="B189" s="1">
+        <v>34682</v>
+      </c>
+      <c r="C189">
+        <v>7.3176470588235301</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>28</v>
+      </c>
+      <c r="B190" s="1">
+        <v>34687</v>
+      </c>
+      <c r="C190">
+        <v>7.9058823529411768</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>28</v>
+      </c>
+      <c r="B191" s="1">
+        <v>34690</v>
+      </c>
+      <c r="C191">
+        <v>7.9411764705882355</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>29</v>
+      </c>
+      <c r="B192" s="1">
+        <v>34605</v>
+      </c>
+      <c r="C192">
+        <v>1.7250000000000003</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>29</v>
+      </c>
+      <c r="B193" s="1">
+        <v>34612</v>
+      </c>
+      <c r="C193">
+        <v>2.2800000000000002</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>29</v>
+      </c>
+      <c r="B194" s="1">
+        <v>34619</v>
+      </c>
+      <c r="C194">
+        <v>3.4049999999999998</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>29</v>
+      </c>
+      <c r="B195" s="1">
+        <v>34626</v>
+      </c>
+      <c r="C195">
+        <v>4.169999999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>29</v>
+      </c>
+      <c r="B196" s="1">
+        <v>34634</v>
+      </c>
+      <c r="C196">
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>29</v>
+      </c>
+      <c r="B197" s="1">
+        <v>34640</v>
+      </c>
+      <c r="C197">
+        <v>6.3449999999999998</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>29</v>
+      </c>
+      <c r="B198" s="1">
+        <v>34645</v>
+      </c>
+      <c r="C198">
+        <v>7.3894736842105262</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>29</v>
+      </c>
+      <c r="B199" s="1">
+        <v>34648</v>
+      </c>
+      <c r="C199">
+        <v>8.0052631578947384</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>29</v>
+      </c>
+      <c r="B200" s="1">
+        <v>34652</v>
+      </c>
+      <c r="C200">
+        <v>8.6105263157894747</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>29</v>
+      </c>
+      <c r="B201" s="1">
+        <v>34655</v>
+      </c>
+      <c r="C201">
+        <v>9.235294117647058</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>29</v>
+      </c>
+      <c r="B202" s="1">
+        <v>34659</v>
+      </c>
+      <c r="C202">
+        <v>9.7764705882352914</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>29</v>
+      </c>
+      <c r="B203" s="1">
+        <v>34662</v>
+      </c>
+      <c r="C203">
+        <v>10.117647058823529</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>30</v>
+      </c>
+      <c r="B204" s="1">
+        <v>34605</v>
+      </c>
+      <c r="C204">
+        <v>1.6850000000000001</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>30</v>
+      </c>
+      <c r="B205" s="1">
+        <v>34612</v>
+      </c>
+      <c r="C205">
+        <v>2.2800000000000002</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>30</v>
+      </c>
+      <c r="B206" s="1">
+        <v>34619</v>
+      </c>
+      <c r="C206">
+        <v>3.3550000000000004</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>30</v>
+      </c>
+      <c r="B207" s="1">
+        <v>34626</v>
+      </c>
+      <c r="C207">
+        <v>4.1549999999999994</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>30</v>
+      </c>
+      <c r="B208" s="1">
+        <v>34634</v>
+      </c>
+      <c r="C208">
+        <v>5.379999999999999</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>30</v>
+      </c>
+      <c r="B209" s="1">
+        <v>34640</v>
+      </c>
+      <c r="C209">
+        <v>6.2150000000000007</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>30</v>
+      </c>
+      <c r="B210" s="1">
+        <v>34645</v>
+      </c>
+      <c r="C210">
+        <v>7.2750000000000004</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>30</v>
+      </c>
+      <c r="B211" s="1">
+        <v>34648</v>
+      </c>
+      <c r="C211">
+        <v>7.7000000000000011</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>30</v>
+      </c>
+      <c r="B212" s="1">
+        <v>34652</v>
+      </c>
+      <c r="C212">
+        <v>8.1900000000000013</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>30</v>
+      </c>
+      <c r="B213" s="1">
+        <v>34655</v>
+      </c>
+      <c r="C213">
+        <v>8.4499999999999993</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>31</v>
+      </c>
+      <c r="B214" s="1">
+        <v>34565</v>
+      </c>
+      <c r="C214">
+        <v>2.165</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>31</v>
+      </c>
+      <c r="B215" s="1">
+        <v>34578</v>
+      </c>
+      <c r="C215">
+        <v>3.105</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>31</v>
+      </c>
+      <c r="B216" s="1">
+        <v>34586</v>
+      </c>
+      <c r="C216">
+        <v>3.7299999999999995</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>31</v>
+      </c>
+      <c r="B217" s="1">
+        <v>34598</v>
+      </c>
+      <c r="C217">
+        <v>4.7949999999999999</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>31</v>
+      </c>
+      <c r="B218" s="1">
+        <v>34605</v>
+      </c>
+      <c r="C218">
+        <v>5.3100000000000005</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>31</v>
+      </c>
+      <c r="B219" s="1">
+        <v>34612</v>
+      </c>
+      <c r="C219">
+        <v>5.9349999999999996</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>31</v>
+      </c>
+      <c r="B220" s="1">
+        <v>34619</v>
+      </c>
+      <c r="C220">
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>31</v>
+      </c>
+      <c r="B221" s="1">
+        <v>34626</v>
+      </c>
+      <c r="C221">
+        <v>7.4650000000000016</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>31</v>
+      </c>
+      <c r="B222" s="1">
+        <v>34634</v>
+      </c>
+      <c r="C222">
+        <v>8.41</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>31</v>
+      </c>
+      <c r="B223" s="1">
+        <v>34640</v>
+      </c>
+      <c r="C223">
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>31</v>
+      </c>
+      <c r="B224" s="1">
+        <v>34645</v>
+      </c>
+      <c r="C224">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>32</v>
+      </c>
+      <c r="B225" s="1">
+        <v>34565</v>
+      </c>
+      <c r="C225">
+        <v>2.0150000000000006</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>32</v>
+      </c>
+      <c r="B226" s="1">
+        <v>34578</v>
+      </c>
+      <c r="C226">
+        <v>2.9450000000000003</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>32</v>
+      </c>
+      <c r="B227" s="1">
+        <v>34586</v>
+      </c>
+      <c r="C227">
+        <v>3.5450000000000004</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>32</v>
+      </c>
+      <c r="B228" s="1">
+        <v>34598</v>
+      </c>
+      <c r="C228">
+        <v>4.5149999999999997</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>32</v>
+      </c>
+      <c r="B229" s="1">
+        <v>34605</v>
+      </c>
+      <c r="C229">
+        <v>5.1049999999999995</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>32</v>
+      </c>
+      <c r="B230" s="1">
+        <v>34612</v>
+      </c>
+      <c r="C230">
+        <v>5.7450000000000001</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>32</v>
+      </c>
+      <c r="B231" s="1">
+        <v>34619</v>
+      </c>
+      <c r="C231">
+        <v>6.6950000000000003</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>32</v>
+      </c>
+      <c r="B232" s="1">
+        <v>34626</v>
+      </c>
+      <c r="C232">
+        <v>7.3399999999999981</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>32</v>
+      </c>
+      <c r="B233" s="1">
+        <v>34634</v>
+      </c>
+      <c r="C233">
+        <v>8.254999999999999</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>32</v>
+      </c>
+      <c r="B234" s="1">
+        <v>34640</v>
+      </c>
+      <c r="C234">
+        <v>9.0299999999999994</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>32</v>
+      </c>
+      <c r="B235" s="1">
+        <v>34645</v>
+      </c>
+      <c r="C235">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>33</v>
+      </c>
+      <c r="B236" s="1">
+        <v>34443</v>
+      </c>
+      <c r="C236">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>33</v>
+      </c>
+      <c r="B237" s="1">
+        <v>34449</v>
+      </c>
+      <c r="C237">
+        <v>1.6799999999999997</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>33</v>
+      </c>
+      <c r="B238" s="1">
+        <v>34458</v>
+      </c>
+      <c r="C238">
+        <v>2.6350000000000002</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>33</v>
+      </c>
+      <c r="B239" s="1">
+        <v>34469</v>
+      </c>
+      <c r="C239">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>33</v>
+      </c>
+      <c r="B240" s="1">
+        <v>34479</v>
+      </c>
+      <c r="C240">
+        <v>4.9049999999999994</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>33</v>
+      </c>
+      <c r="B241" s="1">
+        <v>34486</v>
+      </c>
+      <c r="C241">
+        <v>5.6049999999999986</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>33</v>
+      </c>
+      <c r="B242" s="1">
+        <v>34498</v>
+      </c>
+      <c r="C242">
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>33</v>
+      </c>
+      <c r="B243" s="1">
+        <v>34516</v>
+      </c>
+      <c r="C243">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>33</v>
+      </c>
+      <c r="B244" s="1">
+        <v>34529</v>
+      </c>
+      <c r="C244">
+        <v>7.2299999999999995</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>33</v>
+      </c>
+      <c r="B245" s="1">
+        <v>34544</v>
+      </c>
+      <c r="C245">
+        <v>7.9099999999999993</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>33</v>
+      </c>
+      <c r="B246" s="1">
+        <v>34557</v>
+      </c>
+      <c r="C246">
+        <v>8.6949999999999985</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>33</v>
+      </c>
+      <c r="B247" s="1">
+        <v>34565</v>
+      </c>
+      <c r="C247">
+        <v>9.0400000000000027</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>33</v>
+      </c>
+      <c r="B248" s="1">
+        <v>34578</v>
+      </c>
+      <c r="C248">
+        <v>9.870000000000001</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>33</v>
+      </c>
+      <c r="B249" s="1">
+        <v>34586</v>
+      </c>
+      <c r="C249">
+        <v>10.285</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>33</v>
+      </c>
+      <c r="B250" s="1">
+        <v>34598</v>
+      </c>
+      <c r="C250">
+        <v>11.214999999999998</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>33</v>
+      </c>
+      <c r="B251" s="1">
+        <v>34605</v>
+      </c>
+      <c r="C251">
+        <v>11.654999999999998</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>33</v>
+      </c>
+      <c r="B252" s="1">
+        <v>34612</v>
+      </c>
+      <c r="C252">
+        <v>11.969999999999999</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>33</v>
+      </c>
+      <c r="B253" s="1">
+        <v>34619</v>
+      </c>
+      <c r="C253">
+        <v>12.604999999999997</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>33</v>
+      </c>
+      <c r="B254" s="1">
+        <v>34626</v>
+      </c>
+      <c r="C254">
+        <v>13.02</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>33</v>
+      </c>
+      <c r="B255" s="1">
+        <v>34634</v>
+      </c>
+      <c r="C255">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>34</v>
+      </c>
+      <c r="B256" s="1">
+        <v>34486</v>
+      </c>
+      <c r="C256">
+        <v>4.7210526315789476</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>34</v>
+      </c>
+      <c r="B257" s="1">
+        <v>34498</v>
+      </c>
+      <c r="C257">
+        <v>5.284210526315789</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>34</v>
+      </c>
+      <c r="B258" s="1">
+        <v>34516</v>
+      </c>
+      <c r="C258">
+        <v>5.9105263157894736</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>34</v>
+      </c>
+      <c r="B259" s="1">
+        <v>34529</v>
+      </c>
+      <c r="C259">
+        <v>6.3052631578947365</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>34</v>
+      </c>
+      <c r="B260" s="1">
+        <v>34544</v>
+      </c>
+      <c r="C260">
+        <v>6.889473684210528</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>34</v>
+      </c>
+      <c r="B261" s="1">
+        <v>34557</v>
+      </c>
+      <c r="C261">
+        <v>7.6052631578947354</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>34</v>
+      </c>
+      <c r="B262" s="1">
+        <v>34565</v>
+      </c>
+      <c r="C262">
+        <v>8.0473684210526315</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>34</v>
+      </c>
+      <c r="B263" s="1">
+        <v>34578</v>
+      </c>
+      <c r="C263">
+        <v>8.8842105263157922</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>34</v>
+      </c>
+      <c r="B264" s="1">
+        <v>34586</v>
+      </c>
+      <c r="C264">
+        <v>9.3368421052631607</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>34</v>
+      </c>
+      <c r="B265" s="1">
+        <v>34598</v>
+      </c>
+      <c r="C265">
+        <v>10.178947368421051</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>34</v>
+      </c>
+      <c r="B266" s="1">
+        <v>34605</v>
+      </c>
+      <c r="C266">
+        <v>10.526315789473683</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>34</v>
+      </c>
+      <c r="B267" s="1">
+        <v>34612</v>
+      </c>
+      <c r="C267">
+        <v>10.826315789473687</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>34</v>
+      </c>
+      <c r="B268" s="1">
+        <v>34619</v>
+      </c>
+      <c r="C268">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>34</v>
+      </c>
+      <c r="B269" s="1">
+        <v>34626</v>
+      </c>
+      <c r="C269">
+        <v>11.368421052631579</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>26</v>
+      </c>
+      <c r="E270" s="2">
+        <v>7.2625000000000002</v>
+      </c>
+      <c r="F270" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>28</v>
+      </c>
+      <c r="E271" s="3">
+        <v>7.9411764705882355</v>
+      </c>
+      <c r="F271" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>30</v>
+      </c>
+      <c r="E272" s="3">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="F272" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>32</v>
+      </c>
+      <c r="E273" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="F273" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>34</v>
+      </c>
+      <c r="E274" s="3">
+        <v>11.368421052631579</v>
+      </c>
+      <c r="F274" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>25</v>
+      </c>
+      <c r="E275" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="F275" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>27</v>
+      </c>
+      <c r="E276" s="3">
+        <v>15.714285714285714</v>
+      </c>
+      <c r="F276" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>29</v>
+      </c>
+      <c r="E277" s="3">
+        <v>10.117647058823529</v>
+      </c>
+      <c r="F277" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>31</v>
+      </c>
+      <c r="E278" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F278" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>33</v>
+      </c>
+      <c r="E279" s="4">
+        <v>13.1</v>
+      </c>
+      <c r="F279" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B281" s="5"/>
+      <c r="C281" s="6"/>
+      <c r="F281" s="7"/>
+      <c r="G281" s="2"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B282" s="5"/>
+      <c r="C282" s="8"/>
+      <c r="F282" s="7"/>
+      <c r="G282" s="3"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B283" s="5"/>
+      <c r="C283" s="8"/>
+      <c r="F283" s="7"/>
+      <c r="G283" s="3"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B284" s="5"/>
+      <c r="C284" s="8"/>
+      <c r="F284" s="7"/>
+      <c r="G284" s="3"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B285" s="5"/>
+      <c r="C285" s="8"/>
+      <c r="F285" s="7"/>
+      <c r="G285" s="3"/>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B286" s="5"/>
+      <c r="C286" s="6"/>
+      <c r="F286" s="7"/>
+      <c r="G286" s="2"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B287" s="5"/>
+      <c r="C287" s="8"/>
+      <c r="F287" s="7"/>
+      <c r="G287" s="3"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B288" s="5"/>
+      <c r="C288" s="8"/>
+      <c r="F288" s="7"/>
+      <c r="G288" s="3"/>
+    </row>
+    <row r="289" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B289" s="5"/>
+      <c r="C289" s="8"/>
+      <c r="F289" s="7"/>
+      <c r="G289" s="3"/>
+    </row>
+    <row r="290" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B290" s="5"/>
+      <c r="C290" s="9"/>
+      <c r="F290" s="7"/>
+      <c r="G290" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new Lincoln data
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/PalmerstonNorth1989.xlsx
+++ b/Tests/Validation/Wheat/PalmerstonNorth1989.xlsx
@@ -101,34 +101,34 @@
     <t>PalmerstonNorth1989Sow5-AprCultivarRongotea</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow22-DecCultivarBattenWinter</t>
+    <t>Lincoln1994Sow22-DecCultivarBattenWinter</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow22-DecCultivarBattenSpring</t>
+    <t>Lincoln1994Sow22-DecCultivarBattenSpring</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow27-OctCultivarBattenWinter</t>
+    <t>Lincoln1994Sow27-OctCultivarBattenWinter</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow27-OctCultivarBattenSpring</t>
+    <t>Lincoln1994Sow27-OctCultivarBattenSpring</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow1-SepCultivarBattenWinter</t>
+    <t>Lincoln1994Sow1-SepCultivarBattenWinter</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow1-SepCultivarBattenSpring</t>
+    <t>Lincoln1994Sow1-SepCultivarBattenSpring</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow20-JunCultivarBattenWinter</t>
+    <t>Lincoln1994Sow20-JunCultivarBattenWinter</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow20-JunCultivarBattenSpring</t>
+    <t>Lincoln1994Sow20-JunCultivarBattenSpring</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow5-AprCultivarBattenWinter</t>
+    <t>Lincoln1994Sow5-AprCultivarBattenWinter</t>
   </si>
   <si>
-    <t>PalmerstonNorth1994Sow5-AprCultivarBattenSpring</t>
+    <t>Lincoln1994Sow5-AprCultivarBattenSpring</t>
   </si>
 </sst>
 </file>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B281" sqref="B281:G290"/>
+    <sheetView tabSelected="1" topLeftCell="A221" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Renamed Wheat.Leaf.Height column to LeafHeight
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/PalmerstonNorth1989.xlsx
+++ b/Tests/Validation/Wheat/PalmerstonNorth1989.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhe00a\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F768A893-7542-4DCE-A06B-BDE451DCC3FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8008B778-AC3C-47F6-9D22-E0604D40A9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="30" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Wheat.Phenology.HaunStage</t>
-  </si>
-  <si>
-    <t>Wheat.Leaf.Height</t>
   </si>
   <si>
     <t>Wheat.Phenology.FinalLeafNumber</t>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Lincoln1994Sow5-AprCvBattenSpring</t>
+  </si>
+  <si>
+    <t>LeafHeight</t>
   </si>
 </sst>
 </file>
@@ -244,9 +244,9 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -534,17 +534,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A243" sqref="A243"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,18 +556,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>32686</v>
@@ -578,9 +579,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <v>32686</v>
@@ -592,9 +593,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>32686</v>
@@ -606,9 +607,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>32696</v>
@@ -620,9 +621,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>32696</v>
@@ -634,9 +635,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>32696</v>
@@ -648,9 +649,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>32709</v>
@@ -662,9 +663,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>32709</v>
@@ -676,9 +677,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>32709</v>
@@ -690,9 +691,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1">
         <v>32721</v>
@@ -704,9 +705,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1">
         <v>32721</v>
@@ -718,9 +719,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1">
         <v>32721</v>
@@ -732,9 +733,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1">
         <v>32731</v>
@@ -746,9 +747,9 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1">
         <v>32731</v>
@@ -760,9 +761,9 @@
         <v>8.8333333333333339</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1">
         <v>32731</v>
@@ -774,9 +775,9 @@
         <v>3.1666666666666665</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1">
         <v>32742</v>
@@ -788,9 +789,9 @@
         <v>3.1666666666666665</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1">
         <v>32742</v>
@@ -802,9 +803,9 @@
         <v>31.833333333333332</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1">
         <v>32742</v>
@@ -816,9 +817,9 @@
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1">
         <v>32756</v>
@@ -830,9 +831,9 @@
         <v>13.833333333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1">
         <v>32756</v>
@@ -844,9 +845,9 @@
         <v>130.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1">
         <v>32756</v>
@@ -858,9 +859,9 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1">
         <v>32750</v>
@@ -872,9 +873,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1">
         <v>32750</v>
@@ -886,9 +887,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1">
         <v>32750</v>
@@ -900,9 +901,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1">
         <v>32764</v>
@@ -914,9 +915,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1">
         <v>32764</v>
@@ -928,9 +929,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1">
         <v>32764</v>
@@ -942,9 +943,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1">
         <v>32773</v>
@@ -956,9 +957,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="1">
         <v>32773</v>
@@ -970,9 +971,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" s="1">
         <v>32773</v>
@@ -984,9 +985,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32" s="1">
         <v>32783</v>
@@ -998,9 +999,9 @@
         <v>23.333333333333332</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" s="1">
         <v>32783</v>
@@ -1012,9 +1013,9 @@
         <v>110.5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="1">
         <v>32783</v>
@@ -1026,9 +1027,9 @@
         <v>33.166666666666664</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" s="1">
         <v>32791</v>
@@ -1040,9 +1041,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" s="1">
         <v>32791</v>
@@ -1054,9 +1055,9 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" s="1">
         <v>32791</v>
@@ -1068,9 +1069,9 @@
         <v>76.333333333333329</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" s="1">
         <v>32800</v>
@@ -1082,9 +1083,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" s="1">
         <v>32800</v>
@@ -1096,9 +1097,9 @@
         <v>323.33333333333331</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" s="1">
         <v>32800</v>
@@ -1110,9 +1111,9 @@
         <v>144.83333333333334</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B41" s="1">
         <v>32787</v>
@@ -1124,9 +1125,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42" s="1">
         <v>32787</v>
@@ -1138,9 +1139,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B43" s="1">
         <v>32787</v>
@@ -1152,9 +1153,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B44" s="1">
         <v>32798</v>
@@ -1166,9 +1167,9 @@
         <v>1.1666666666666667</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B45" s="1">
         <v>32798</v>
@@ -1180,9 +1181,9 @@
         <v>10.333333333333334</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B46" s="1">
         <v>32798</v>
@@ -1194,9 +1195,9 @@
         <v>8.1666666666666661</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B47" s="1">
         <v>32806</v>
@@ -1208,9 +1209,9 @@
         <v>9.8333333333333339</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B48" s="1">
         <v>32806</v>
@@ -1222,9 +1223,9 @@
         <v>29.166666666666668</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B49" s="1">
         <v>32806</v>
@@ -1236,9 +1237,9 @@
         <v>21.166666666666668</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B50" s="1">
         <v>32813</v>
@@ -1250,9 +1251,9 @@
         <v>36.833333333333336</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B51" s="1">
         <v>32813</v>
@@ -1264,9 +1265,9 @@
         <v>78.333333333333329</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B52" s="1">
         <v>32813</v>
@@ -1278,9 +1279,9 @@
         <v>52.333333333333336</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B53" s="1">
         <v>32825</v>
@@ -1292,9 +1293,9 @@
         <v>147.16666666666666</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54" s="1">
         <v>32825</v>
@@ -1306,9 +1307,9 @@
         <v>240</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B55" s="1">
         <v>32825</v>
@@ -1320,9 +1321,9 @@
         <v>154.16666666666666</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B56" s="1">
         <v>32849</v>
@@ -1334,9 +1335,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B57" s="1">
         <v>32849</v>
@@ -1348,9 +1349,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B58" s="1">
         <v>32849</v>
@@ -1362,9 +1363,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B59" s="1">
         <v>32856</v>
@@ -1376,9 +1377,9 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B60" s="1">
         <v>32856</v>
@@ -1390,9 +1391,9 @@
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B61" s="1">
         <v>32856</v>
@@ -1404,9 +1405,9 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B62" s="1">
         <v>32862</v>
@@ -1418,9 +1419,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B63" s="1">
         <v>32862</v>
@@ -1432,9 +1433,9 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64" s="1">
         <v>32862</v>
@@ -1446,9 +1447,9 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B65" s="1">
         <v>32868</v>
@@ -1460,9 +1461,9 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B66" s="1">
         <v>32868</v>
@@ -1474,9 +1475,9 @@
         <v>42.833333333333336</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B67" s="1">
         <v>32868</v>
@@ -1488,9 +1489,9 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B68" s="1">
         <v>32878</v>
@@ -1502,9 +1503,9 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B69" s="1">
         <v>32878</v>
@@ -1516,9 +1517,9 @@
         <v>160.83333333333334</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B70" s="1">
         <v>32878</v>
@@ -1530,9 +1531,9 @@
         <v>126.83333333333333</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B71" s="1">
         <v>32937</v>
@@ -1544,9 +1545,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B72" s="1">
         <v>32937</v>
@@ -1558,9 +1559,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B73" s="1">
         <v>32937</v>
@@ -1572,9 +1573,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B74" s="1">
         <v>32941</v>
@@ -1586,9 +1587,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B75" s="1">
         <v>32941</v>
@@ -1600,9 +1601,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B76" s="1">
         <v>32941</v>
@@ -1614,9 +1615,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B77" s="1">
         <v>32945</v>
@@ -1628,9 +1629,9 @@
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B78" s="1">
         <v>32945</v>
@@ -1642,9 +1643,9 @@
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B79" s="1">
         <v>32945</v>
@@ -1656,9 +1657,9 @@
         <v>4.333333333333333</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B80" s="1">
         <v>32948</v>
@@ -1670,9 +1671,9 @@
         <v>3.1666666666666665</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B81" s="1">
         <v>32948</v>
@@ -1684,9 +1685,9 @@
         <v>9.6666666666666661</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B82" s="1">
         <v>32948</v>
@@ -1698,9 +1699,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B83" s="1">
         <v>32954</v>
@@ -1712,9 +1713,9 @@
         <v>3.8333333333333335</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B84" s="1">
         <v>32954</v>
@@ -1726,9 +1727,9 @@
         <v>27.666666666666668</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B85" s="1">
         <v>32954</v>
@@ -1740,9 +1741,9 @@
         <v>8.1666666666666661</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B86" s="1">
         <v>32959</v>
@@ -1754,9 +1755,9 @@
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B87" s="1">
         <v>32959</v>
@@ -1768,9 +1769,9 @@
         <v>49.833333333333336</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B88" s="1">
         <v>32959</v>
@@ -1782,9 +1783,9 @@
         <v>13.333333333333334</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B89" s="1">
         <v>32965</v>
@@ -1796,9 +1797,9 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B90" s="1">
         <v>32965</v>
@@ -1810,9 +1811,9 @@
         <v>125.66666666666667</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B91" s="1">
         <v>32965</v>
@@ -1824,9 +1825,9 @@
         <v>26.333333333333332</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B92" s="1">
         <v>32973</v>
@@ -1838,9 +1839,9 @@
         <v>26.666666666666668</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B93" s="1">
         <v>32973</v>
@@ -1852,9 +1853,9 @@
         <v>207.5</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B94" s="1">
         <v>32973</v>
@@ -1866,9 +1867,9 @@
         <v>45.833333333333336</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B95" s="1">
         <v>32983</v>
@@ -1880,9 +1881,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B96" s="1">
         <v>32983</v>
@@ -1894,9 +1895,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B97" s="1">
         <v>32983</v>
@@ -1908,9 +1909,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B98" s="1">
         <v>32990</v>
@@ -1922,9 +1923,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B99" s="1">
         <v>32990</v>
@@ -1936,9 +1937,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B100" s="1">
         <v>32990</v>
@@ -1950,9 +1951,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B101" s="1">
         <v>32997</v>
@@ -1964,9 +1965,9 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B102" s="1">
         <v>32997</v>
@@ -1978,9 +1979,9 @@
         <v>6.166666666666667</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B103" s="1">
         <v>32997</v>
@@ -1992,9 +1993,9 @@
         <v>3.1666666666666665</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B104" s="1">
         <v>33004</v>
@@ -2006,9 +2007,9 @@
         <v>4.166666666666667</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B105" s="1">
         <v>33004</v>
@@ -2020,9 +2021,9 @@
         <v>9.6666666666666661</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B106" s="1">
         <v>33004</v>
@@ -2034,9 +2035,9 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B107" s="1">
         <v>33014</v>
@@ -2048,9 +2049,9 @@
         <v>6.166666666666667</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B108" s="1">
         <v>33014</v>
@@ -2062,9 +2063,9 @@
         <v>50.166666666666664</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B109" s="1">
         <v>33014</v>
@@ -2076,9 +2077,9 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B110" s="1">
         <v>33023</v>
@@ -2090,9 +2091,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B111" s="1">
         <v>33023</v>
@@ -2104,9 +2105,9 @@
         <v>113.66666666666667</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B112" s="1">
         <v>33023</v>
@@ -2118,9 +2119,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B113" s="1">
         <v>33035</v>
@@ -2132,9 +2133,9 @@
         <v>34.833333333333336</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B114" s="1">
         <v>33035</v>
@@ -2146,9 +2147,9 @@
         <v>204.16666666666666</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B115" s="1">
         <v>33035</v>
@@ -2160,9 +2161,9 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B116" s="1">
         <v>33052</v>
@@ -2174,9 +2175,9 @@
         <v>65.833333333333329</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B117" s="1">
         <v>33052</v>
@@ -2188,9 +2189,9 @@
         <v>305.83333333333331</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B118" s="1">
         <v>33052</v>
@@ -2202,207 +2203,207 @@
         <v>108.33333333333333</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E119">
         <v>10.933333333333334</v>
       </c>
       <c r="F119" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E120">
         <v>10</v>
       </c>
       <c r="F120" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E121">
         <v>8.1999999999999993</v>
       </c>
       <c r="F121" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E122">
         <v>7.666666666666667</v>
       </c>
       <c r="F122" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E123">
         <v>9.8666666666666671</v>
       </c>
       <c r="F123" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E124">
         <v>11.666666666666666</v>
       </c>
       <c r="F124" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E125">
         <v>9.0666666666666664</v>
       </c>
       <c r="F125" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E126">
         <v>8.2666666666666675</v>
       </c>
       <c r="F126" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E127">
         <v>7.4</v>
       </c>
       <c r="F127" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E128">
         <v>7.1333333333333337</v>
       </c>
       <c r="F128" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E129">
         <v>7.2666666666666666</v>
       </c>
       <c r="F129" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E130">
         <v>8.2666666666666675</v>
       </c>
       <c r="F130" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E131">
         <v>10.6</v>
       </c>
       <c r="F131" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E132">
         <v>9.7333333333333325</v>
       </c>
       <c r="F132" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E133">
         <v>8.4666666666666668</v>
       </c>
       <c r="F133" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E134">
         <v>7.666666666666667</v>
       </c>
       <c r="F134" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E135">
         <v>9.5333333333333332</v>
       </c>
       <c r="F135" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E136">
         <v>11.2</v>
       </c>
       <c r="F136" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B137" s="1">
         <v>34704</v>
@@ -2411,9 +2412,9 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B138" s="1">
         <v>34711</v>
@@ -2422,9 +2423,9 @@
         <v>3.0500000000000003</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B139" s="1">
         <v>34715</v>
@@ -2433,9 +2434,9 @@
         <v>3.8899999999999997</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B140" s="1">
         <v>34718</v>
@@ -2444,9 +2445,9 @@
         <v>4.3650000000000002</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B141" s="1">
         <v>34723</v>
@@ -2455,9 +2456,9 @@
         <v>5.0631578947368414</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B142" s="1">
         <v>34725</v>
@@ -2466,9 +2467,9 @@
         <v>5.7312500000000002</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B143" s="1">
         <v>34729</v>
@@ -2477,9 +2478,9 @@
         <v>6.3812499999999988</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B144" s="1">
         <v>34733</v>
@@ -2488,9 +2489,9 @@
         <v>6.9866666666666664</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B145" s="1">
         <v>34737</v>
@@ -2499,9 +2500,9 @@
         <v>7.5866666666666669</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B146" s="1">
         <v>34740</v>
@@ -2510,9 +2511,9 @@
         <v>8.06</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B147" s="1">
         <v>34744</v>
@@ -2521,9 +2522,9 @@
         <v>8.7066666666666688</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B148" s="1">
         <v>34751</v>
@@ -2532,9 +2533,9 @@
         <v>9.7714285714285705</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B149" s="1">
         <v>34754</v>
@@ -2543,9 +2544,9 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B150" s="1">
         <v>34759</v>
@@ -2554,9 +2555,9 @@
         <v>10.592857142857143</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B151" s="1">
         <v>34765</v>
@@ -2565,9 +2566,9 @@
         <v>11.142857142857144</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B152" s="1">
         <v>34775</v>
@@ -2576,9 +2577,9 @@
         <v>12.035714285714286</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B153" s="1">
         <v>34785</v>
@@ -2587,9 +2588,9 @@
         <v>12.958333333333334</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B154" s="1">
         <v>34799</v>
@@ -2598,9 +2599,9 @@
         <v>14.246153846153845</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B155" s="1">
         <v>34807</v>
@@ -2609,9 +2610,9 @@
         <v>14.899999999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B156" s="1">
         <v>34829</v>
@@ -2620,9 +2621,9 @@
         <v>16.683333333333334</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B157" s="1">
         <v>34838</v>
@@ -2631,9 +2632,9 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B158" s="1">
         <v>34704</v>
@@ -2642,9 +2643,9 @@
         <v>1.8249999999999997</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B159" s="1">
         <v>34711</v>
@@ -2653,9 +2654,9 @@
         <v>3.1450000000000005</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B160" s="1">
         <v>34715</v>
@@ -2664,9 +2665,9 @@
         <v>4.0349999999999993</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B161" s="1">
         <v>34718</v>
@@ -2675,9 +2676,9 @@
         <v>4.4999999999999991</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B162" s="1">
         <v>34723</v>
@@ -2686,9 +2687,9 @@
         <v>5.83</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B163" s="1">
         <v>34725</v>
@@ -2697,9 +2698,9 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B164" s="1">
         <v>34729</v>
@@ -2708,9 +2709,9 @@
         <v>6.5421052631578949</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B165" s="1">
         <v>34733</v>
@@ -2719,9 +2720,9 @@
         <v>6.9555555555555557</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B166" s="1">
         <v>34737</v>
@@ -2730,9 +2731,9 @@
         <v>7.2625000000000002</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B167" s="1">
         <v>34655</v>
@@ -2741,9 +2742,9 @@
         <v>2.9450000000000003</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B168" s="1">
         <v>34659</v>
@@ -2752,9 +2753,9 @@
         <v>3.5450000000000004</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B169" s="1">
         <v>34662</v>
@@ -2763,9 +2764,9 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B170" s="1">
         <v>34666</v>
@@ -2774,9 +2775,9 @@
         <v>4.9949999999999992</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B171" s="1">
         <v>34669</v>
@@ -2785,9 +2786,9 @@
         <v>5.4950000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B172" s="1">
         <v>34675</v>
@@ -2796,9 +2797,9 @@
         <v>6.7117647058823522</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B173" s="1">
         <v>34682</v>
@@ -2807,9 +2808,9 @@
         <v>7.7529411764705873</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B174" s="1">
         <v>34687</v>
@@ -2818,9 +2819,9 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B175" s="1">
         <v>34690</v>
@@ -2829,9 +2830,9 @@
         <v>9.4764705882352906</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B176" s="1">
         <v>34694</v>
@@ -2840,9 +2841,9 @@
         <v>10.013333333333334</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B177" s="1">
         <v>34697</v>
@@ -2851,9 +2852,9 @@
         <v>10.45</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B178" s="1">
         <v>34701</v>
@@ -2862,9 +2863,9 @@
         <v>11.015384615384615</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B179" s="1">
         <v>34704</v>
@@ -2873,9 +2874,9 @@
         <v>11.266666666666666</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B180" s="1">
         <v>34711</v>
@@ -2884,9 +2885,9 @@
         <v>12.033333333333333</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B181" s="1">
         <v>34725</v>
@@ -2895,9 +2896,9 @@
         <v>14.455555555555557</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B182" s="1">
         <v>34733</v>
@@ -2906,9 +2907,9 @@
         <v>15.714285714285714</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B183" s="1">
         <v>34655</v>
@@ -2917,9 +2918,9 @@
         <v>2.6949999999999998</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B184" s="1">
         <v>34659</v>
@@ -2928,9 +2929,9 @@
         <v>3.2789473684210524</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B185" s="1">
         <v>34662</v>
@@ -2939,9 +2940,9 @@
         <v>3.8249999999999993</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B186" s="1">
         <v>34666</v>
@@ -2950,9 +2951,9 @@
         <v>4.7150000000000007</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B187" s="1">
         <v>34669</v>
@@ -2961,9 +2962,9 @@
         <v>5.1850000000000005</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B188" s="1">
         <v>34675</v>
@@ -2972,9 +2973,9 @@
         <v>6.2111111111111112</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B189" s="1">
         <v>34682</v>
@@ -2983,9 +2984,9 @@
         <v>7.3176470588235301</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B190" s="1">
         <v>34687</v>
@@ -2994,9 +2995,9 @@
         <v>7.9058823529411768</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B191" s="1">
         <v>34690</v>
@@ -3005,9 +3006,9 @@
         <v>7.9411764705882355</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B192" s="1">
         <v>34605</v>
@@ -3016,9 +3017,9 @@
         <v>1.7250000000000003</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B193" s="1">
         <v>34612</v>
@@ -3027,9 +3028,9 @@
         <v>2.2800000000000002</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B194" s="1">
         <v>34619</v>
@@ -3038,9 +3039,9 @@
         <v>3.4049999999999998</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B195" s="1">
         <v>34626</v>
@@ -3049,9 +3050,9 @@
         <v>4.169999999999999</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B196" s="1">
         <v>34634</v>
@@ -3060,9 +3061,9 @@
         <v>5.41</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B197" s="1">
         <v>34640</v>
@@ -3071,9 +3072,9 @@
         <v>6.3449999999999998</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B198" s="1">
         <v>34645</v>
@@ -3082,9 +3083,9 @@
         <v>7.3894736842105262</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B199" s="1">
         <v>34648</v>
@@ -3093,9 +3094,9 @@
         <v>8.0052631578947384</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B200" s="1">
         <v>34652</v>
@@ -3104,9 +3105,9 @@
         <v>8.6105263157894747</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B201" s="1">
         <v>34655</v>
@@ -3115,9 +3116,9 @@
         <v>9.235294117647058</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B202" s="1">
         <v>34659</v>
@@ -3126,9 +3127,9 @@
         <v>9.7764705882352914</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B203" s="1">
         <v>34662</v>
@@ -3137,9 +3138,9 @@
         <v>10.117647058823529</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B204" s="1">
         <v>34605</v>
@@ -3148,9 +3149,9 @@
         <v>1.6850000000000001</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B205" s="1">
         <v>34612</v>
@@ -3159,9 +3160,9 @@
         <v>2.2800000000000002</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B206" s="1">
         <v>34619</v>
@@ -3170,9 +3171,9 @@
         <v>3.3550000000000004</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B207" s="1">
         <v>34626</v>
@@ -3181,9 +3182,9 @@
         <v>4.1549999999999994</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B208" s="1">
         <v>34634</v>
@@ -3192,9 +3193,9 @@
         <v>5.379999999999999</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B209" s="1">
         <v>34640</v>
@@ -3203,9 +3204,9 @@
         <v>6.2150000000000007</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B210" s="1">
         <v>34645</v>
@@ -3214,9 +3215,9 @@
         <v>7.2750000000000004</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B211" s="1">
         <v>34648</v>
@@ -3225,9 +3226,9 @@
         <v>7.7000000000000011</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B212" s="1">
         <v>34652</v>
@@ -3236,9 +3237,9 @@
         <v>8.1900000000000013</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B213" s="1">
         <v>34655</v>
@@ -3247,9 +3248,9 @@
         <v>8.4499999999999993</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B214" s="1">
         <v>34565</v>
@@ -3258,9 +3259,9 @@
         <v>2.165</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B215" s="1">
         <v>34578</v>
@@ -3269,9 +3270,9 @@
         <v>3.105</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B216" s="1">
         <v>34586</v>
@@ -3280,9 +3281,9 @@
         <v>3.7299999999999995</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B217" s="1">
         <v>34598</v>
@@ -3291,9 +3292,9 @@
         <v>4.7949999999999999</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B218" s="1">
         <v>34605</v>
@@ -3302,9 +3303,9 @@
         <v>5.3100000000000005</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B219" s="1">
         <v>34612</v>
@@ -3313,9 +3314,9 @@
         <v>5.9349999999999996</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B220" s="1">
         <v>34619</v>
@@ -3324,9 +3325,9 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B221" s="1">
         <v>34626</v>
@@ -3335,9 +3336,9 @@
         <v>7.4650000000000016</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B222" s="1">
         <v>34634</v>
@@ -3346,9 +3347,9 @@
         <v>8.41</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B223" s="1">
         <v>34640</v>
@@ -3357,9 +3358,9 @@
         <v>9.09</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B224" s="1">
         <v>34645</v>
@@ -3368,9 +3369,9 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B225" s="1">
         <v>34565</v>
@@ -3379,9 +3380,9 @@
         <v>2.0150000000000006</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B226" s="1">
         <v>34578</v>
@@ -3390,9 +3391,9 @@
         <v>2.9450000000000003</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B227" s="1">
         <v>34586</v>
@@ -3401,9 +3402,9 @@
         <v>3.5450000000000004</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B228" s="1">
         <v>34598</v>
@@ -3412,9 +3413,9 @@
         <v>4.5149999999999997</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B229" s="1">
         <v>34605</v>
@@ -3423,9 +3424,9 @@
         <v>5.1049999999999995</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B230" s="1">
         <v>34612</v>
@@ -3434,9 +3435,9 @@
         <v>5.7450000000000001</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B231" s="1">
         <v>34619</v>
@@ -3445,9 +3446,9 @@
         <v>6.6950000000000003</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B232" s="1">
         <v>34626</v>
@@ -3456,9 +3457,9 @@
         <v>7.3399999999999981</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B233" s="1">
         <v>34634</v>
@@ -3467,9 +3468,9 @@
         <v>8.254999999999999</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B234" s="1">
         <v>34640</v>
@@ -3478,9 +3479,9 @@
         <v>9.0299999999999994</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B235" s="1">
         <v>34645</v>
@@ -3489,9 +3490,9 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B236" s="1">
         <v>34443</v>
@@ -3500,9 +3501,9 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B237" s="1">
         <v>34449</v>
@@ -3511,9 +3512,9 @@
         <v>1.6799999999999997</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B238" s="1">
         <v>34458</v>
@@ -3522,9 +3523,9 @@
         <v>2.6350000000000002</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B239" s="1">
         <v>34469</v>
@@ -3533,9 +3534,9 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B240" s="1">
         <v>34479</v>
@@ -3544,9 +3545,9 @@
         <v>4.9049999999999994</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B241" s="1">
         <v>34486</v>
@@ -3555,9 +3556,9 @@
         <v>5.6049999999999986</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B242" s="1">
         <v>34498</v>
@@ -3566,9 +3567,9 @@
         <v>6.24</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B243" s="1">
         <v>34516</v>
@@ -3577,9 +3578,9 @@
         <v>6.82</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B244" s="1">
         <v>34529</v>
@@ -3588,9 +3589,9 @@
         <v>7.2299999999999995</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B245" s="1">
         <v>34544</v>
@@ -3599,9 +3600,9 @@
         <v>7.9099999999999993</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B246" s="1">
         <v>34557</v>
@@ -3610,9 +3611,9 @@
         <v>8.6949999999999985</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B247" s="1">
         <v>34565</v>
@@ -3621,9 +3622,9 @@
         <v>9.0400000000000027</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B248" s="1">
         <v>34578</v>
@@ -3632,9 +3633,9 @@
         <v>9.870000000000001</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B249" s="1">
         <v>34586</v>
@@ -3643,9 +3644,9 @@
         <v>10.285</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B250" s="1">
         <v>34598</v>
@@ -3654,9 +3655,9 @@
         <v>11.214999999999998</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B251" s="1">
         <v>34605</v>
@@ -3665,9 +3666,9 @@
         <v>11.654999999999998</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B252" s="1">
         <v>34612</v>
@@ -3676,9 +3677,9 @@
         <v>11.969999999999999</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B253" s="1">
         <v>34619</v>
@@ -3687,9 +3688,9 @@
         <v>12.604999999999997</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B254" s="1">
         <v>34626</v>
@@ -3698,9 +3699,9 @@
         <v>13.02</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B255" s="1">
         <v>34634</v>
@@ -3709,9 +3710,9 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B256" s="1">
         <v>34486</v>
@@ -3720,9 +3721,9 @@
         <v>4.7210526315789476</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B257" s="1">
         <v>34498</v>
@@ -3731,9 +3732,9 @@
         <v>5.284210526315789</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B258" s="1">
         <v>34516</v>
@@ -3742,9 +3743,9 @@
         <v>5.9105263157894736</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B259" s="1">
         <v>34529</v>
@@ -3753,9 +3754,9 @@
         <v>6.3052631578947365</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B260" s="1">
         <v>34544</v>
@@ -3764,9 +3765,9 @@
         <v>6.889473684210528</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B261" s="1">
         <v>34557</v>
@@ -3775,9 +3776,9 @@
         <v>7.6052631578947354</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B262" s="1">
         <v>34565</v>
@@ -3786,9 +3787,9 @@
         <v>8.0473684210526315</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B263" s="1">
         <v>34578</v>
@@ -3797,9 +3798,9 @@
         <v>8.8842105263157922</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B264" s="1">
         <v>34586</v>
@@ -3808,9 +3809,9 @@
         <v>9.3368421052631607</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B265" s="1">
         <v>34598</v>
@@ -3819,9 +3820,9 @@
         <v>10.178947368421051</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B266" s="1">
         <v>34605</v>
@@ -3830,9 +3831,9 @@
         <v>10.526315789473683</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B267" s="1">
         <v>34612</v>
@@ -3841,9 +3842,9 @@
         <v>10.826315789473687</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B268" s="1">
         <v>34619</v>
@@ -3852,9 +3853,9 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B269" s="1">
         <v>34626</v>
@@ -3863,171 +3864,171 @@
         <v>11.368421052631579</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E270" s="2">
         <v>7.2625000000000002</v>
       </c>
       <c r="F270" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E271" s="3">
         <v>7.9411764705882355</v>
       </c>
       <c r="F271" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E272" s="3">
         <v>8.4499999999999993</v>
       </c>
       <c r="F272" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E273" s="3">
         <v>9.6</v>
       </c>
       <c r="F273" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E274" s="3">
         <v>11.368421052631579</v>
       </c>
       <c r="F274" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E275" s="2">
         <v>17.2</v>
       </c>
       <c r="F275" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E276" s="3">
         <v>15.714285714285714</v>
       </c>
       <c r="F276" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E277" s="3">
         <v>10.117647058823529</v>
       </c>
       <c r="F277" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E278" s="3">
         <v>9.6999999999999993</v>
       </c>
       <c r="F278" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E279" s="4">
         <v>13.1</v>
       </c>
       <c r="F279" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B281" s="5"/>
       <c r="C281" s="6"/>
       <c r="F281" s="7"/>
       <c r="G281" s="2"/>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B282" s="5"/>
       <c r="C282" s="8"/>
       <c r="F282" s="7"/>
       <c r="G282" s="3"/>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B283" s="5"/>
       <c r="C283" s="8"/>
       <c r="F283" s="7"/>
       <c r="G283" s="3"/>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B284" s="5"/>
       <c r="C284" s="8"/>
       <c r="F284" s="7"/>
       <c r="G284" s="3"/>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B285" s="5"/>
       <c r="C285" s="8"/>
       <c r="F285" s="7"/>
       <c r="G285" s="3"/>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B286" s="5"/>
       <c r="C286" s="6"/>
       <c r="F286" s="7"/>
       <c r="G286" s="2"/>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B287" s="5"/>
       <c r="C287" s="8"/>
       <c r="F287" s="7"/>
       <c r="G287" s="3"/>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B288" s="5"/>
       <c r="C288" s="8"/>
       <c r="F288" s="7"/>
       <c r="G288" s="3"/>
     </row>
-    <row r="289" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="289" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B289" s="5"/>
       <c r="C289" s="8"/>
       <c r="F289" s="7"/>
       <c r="G289" s="3"/>
     </row>
-    <row r="290" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="290" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B290" s="5"/>
       <c r="C290" s="9"/>
       <c r="F290" s="7"/>

</xml_diff>